<commit_message>
Updated Report structure with missing tasks.
</commit_message>
<xml_diff>
--- a/Report/ReportStructure.xlsx
+++ b/Report/ReportStructure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b344b2188dd7c69c/1_Tudelft/Masters/Masters program/SC/Year 1/Q4/Integration Project/Github Project/SC42035-Integration-Project/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{D9E94E44-9945-4B6C-900F-CDE4972BB417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67B3E349-851F-4242-BC5D-00CB53A78893}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{D9E94E44-9945-4B6C-900F-CDE4972BB417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99871B08-19F8-4DE1-870D-0AE85762C53F}"/>
   <bookViews>
-    <workbookView xWindow="-9768" yWindow="5328" windowWidth="17280" windowHeight="9420" xr2:uid="{794B92D1-A42F-4AC0-B166-CAED3B4CB899}"/>
+    <workbookView xWindow="-5556" yWindow="6312" windowWidth="11172" windowHeight="9408" xr2:uid="{794B92D1-A42F-4AC0-B166-CAED3B4CB899}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Introduction</t>
   </si>
@@ -66,6 +66,47 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Extra's</t>
+  </si>
+  <si>
+    <t>Preface</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>review coupling part</t>
+  </si>
+  <si>
+    <t>Bibliography</t>
+  </si>
+  <si>
+    <t>Appendix</t>
+  </si>
+  <si>
+    <t>add models</t>
+  </si>
+  <si>
+    <t>fix missing links</t>
+  </si>
+  <si>
+    <t>add lqr results (check for lqr + initial)
+add result comparison</t>
+  </si>
+  <si>
+    <t>review?</t>
+  </si>
+  <si>
+    <t>check labels
+check consistency</t>
   </si>
 </sst>
 </file>
@@ -109,9 +150,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,96 +472,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D877882-78DD-412F-AF93-C2EE5F9D10EB}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C8" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <f>SUM(B2:B9)</f>
-        <v>29.5</v>
+      <c r="B14">
+        <f>SUM(B2:B13)</f>
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <f>AVERAGE(C2:C13)</f>
+        <v>0.6333333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on report progress.
</commit_message>
<xml_diff>
--- a/Report/ReportStructure.xlsx
+++ b/Report/ReportStructure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b344b2188dd7c69c/1_Tudelft/Masters/Masters program/SC/Year 1/Q4/Integration Project/Github Project/SC42035-Integration-Project/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{D9E94E44-9945-4B6C-900F-CDE4972BB417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99871B08-19F8-4DE1-870D-0AE85762C53F}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{D9E94E44-9945-4B6C-900F-CDE4972BB417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8D61DEC-FA55-44BC-A6DD-92AFBEDFA96D}"/>
   <bookViews>
-    <workbookView xWindow="-5556" yWindow="6312" windowWidth="11172" windowHeight="9408" xr2:uid="{794B92D1-A42F-4AC0-B166-CAED3B4CB899}"/>
+    <workbookView xWindow="0" yWindow="3552" windowWidth="11172" windowHeight="9408" xr2:uid="{794B92D1-A42F-4AC0-B166-CAED3B4CB899}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Introduction</t>
   </si>
@@ -83,19 +83,10 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>review coupling part</t>
-  </si>
-  <si>
     <t>Bibliography</t>
   </si>
   <si>
     <t>Appendix</t>
-  </si>
-  <si>
-    <t>add models</t>
-  </si>
-  <si>
-    <t>fix missing links</t>
   </si>
   <si>
     <t>add lqr results (check for lqr + initial)
@@ -475,7 +466,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,10 +555,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -581,7 +569,7 @@
         <v>0.8</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -606,7 +594,7 @@
         <v>0.5</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -622,30 +610,24 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -658,7 +640,7 @@
       </c>
       <c r="C14" s="2">
         <f>AVERAGE(C2:C13)</f>
-        <v>0.6333333333333333</v>
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -666,7 +648,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to report. + LQR experiment.
</commit_message>
<xml_diff>
--- a/Report/ReportStructure.xlsx
+++ b/Report/ReportStructure.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="87" documentId="8_{D9E94E44-9945-4B6C-900F-CDE4972BB417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8D61DEC-FA55-44BC-A6DD-92AFBEDFA96D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3552" windowWidth="11172" windowHeight="9408" xr2:uid="{794B92D1-A42F-4AC0-B166-CAED3B4CB899}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{794B92D1-A42F-4AC0-B166-CAED3B4CB899}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>